<commit_message>
stable v21 changeover and refresh scan stable
</commit_message>
<xml_diff>
--- a/history-2026-01-30.xlsx
+++ b/history-2026-01-30.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,7 +463,7 @@
         <v>31/01/2026</v>
       </c>
       <c r="B2" t="str">
-        <v>01:42:29</v>
+        <v>01:47:07</v>
       </c>
       <c r="C2" t="str">
         <v>SFG00391</v>
@@ -490,7 +490,7 @@
         <v/>
       </c>
       <c r="K2" t="str">
-        <v>1P1727184121</v>
+        <v>350851-1</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -504,7 +504,7 @@
         <v>31/01/2026</v>
       </c>
       <c r="B3" t="str">
-        <v>01:42:18</v>
+        <v>01:42:29</v>
       </c>
       <c r="C3" t="str">
         <v>SFG00391</v>
@@ -531,7 +531,7 @@
         <v/>
       </c>
       <c r="K3" t="str">
-        <v>350851-1</v>
+        <v>1P1727184121</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -545,7 +545,7 @@
         <v>31/01/2026</v>
       </c>
       <c r="B4" t="str">
-        <v>01:33:34</v>
+        <v>01:42:18</v>
       </c>
       <c r="C4" t="str">
         <v>SFG00391</v>
@@ -572,7 +572,7 @@
         <v/>
       </c>
       <c r="K4" t="str">
-        <v>1P1727184121</v>
+        <v>350851-1</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -586,7 +586,7 @@
         <v>31/01/2026</v>
       </c>
       <c r="B5" t="str">
-        <v>01:33:25</v>
+        <v>01:33:34</v>
       </c>
       <c r="C5" t="str">
         <v>SFG00391</v>
@@ -613,7 +613,7 @@
         <v/>
       </c>
       <c r="K5" t="str">
-        <v>350851-1</v>
+        <v>1P1727184121</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -627,7 +627,7 @@
         <v>31/01/2026</v>
       </c>
       <c r="B6" t="str">
-        <v>01:25:46</v>
+        <v>01:33:25</v>
       </c>
       <c r="C6" t="str">
         <v>SFG00391</v>
@@ -660,12 +660,53 @@
         <v/>
       </c>
       <c r="M6" t="str">
+        <v>ALL_FIELDS_MATCHED</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>31/01/2026</v>
+      </c>
+      <c r="B7" t="str">
+        <v>01:25:46</v>
+      </c>
+      <c r="C7" t="str">
+        <v>SFG00391</v>
+      </c>
+      <c r="D7" t="str">
+        <v>UL1015AWG20WHITE(BARE)</v>
+      </c>
+      <c r="E7" t="str">
+        <v>White</v>
+      </c>
+      <c r="F7" t="str">
+        <v>1470</v>
+      </c>
+      <c r="G7" t="str">
+        <v>1P1727184121</v>
+      </c>
+      <c r="H7" t="str">
+        <v>350851-1</v>
+      </c>
+      <c r="I7" t="str">
+        <v>W11660635</v>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v>350851-1</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
         <v>ALL_FIELDS_MATCHED</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>